<commit_message>
Added Process field in Manual and Bulk Excel
Added Process field in Manual and Bulk Excel
</commit_message>
<xml_diff>
--- a/public/template/Fams_sample_template.xlsx
+++ b/public/template/Fams_sample_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN-SHR\beta\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82CAB45-8F0B-4DA2-B492-6B2296D52B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD0C641-62E3-4949-B59D-F3648F2E6368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>Clean File</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Typing</t>
   </si>
 </sst>
 </file>
@@ -975,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,12 +996,12 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="5" max="7" width="16" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1012,27 +1021,30 @@
         <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45436</v>
       </c>
       <c r="B2" s="1">
-        <v>1213218873</v>
+        <v>1213286</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -1047,27 +1059,30 @@
         <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45439</v>
       </c>
       <c r="B3" s="1">
-        <v>21932183821</v>
+        <v>2193289</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -1082,18 +1097,21 @@
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>